<commit_message>
Labeled the second half of data instances in politics_data_complete.xlsx.
</commit_message>
<xml_diff>
--- a/politics_data_complete.xlsx
+++ b/politics_data_complete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtvar\cs425\CS425SuperVillians\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhett\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ECFD59A-2101-45C3-8548-414AB028EFA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0193CC7A-F0D8-45AE-BA58-0EA3431A6AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="491">
   <si>
     <t>author</t>
   </si>
@@ -1502,6 +1502,9 @@
   </si>
   <si>
     <t>Kappa_scores</t>
+  </si>
+  <si>
+    <t>reliable</t>
   </si>
 </sst>
 </file>
@@ -1782,9 +1785,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1792,10 +1792,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1804,21 +1813,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1828,12 +1828,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2136,10 +2139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC77"/>
+  <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="N10" workbookViewId="0">
+      <selection activeCell="AD39" sqref="AD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2178,7 @@
     <col min="29" max="29" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2260,8 +2263,11 @@
       <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD1" s="5" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2427,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2590,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2670,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2750,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2833,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3153,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3233,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3313,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4777,7 +4783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4857,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4937,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -5017,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -5100,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -5180,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -5263,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -5342,8 +5348,11 @@
       <c r="AC39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -5422,8 +5431,11 @@
       <c r="AC40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -5502,8 +5514,11 @@
       <c r="AC41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -5582,8 +5597,11 @@
       <c r="AC42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -5662,8 +5680,11 @@
       <c r="AC43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -5745,8 +5766,11 @@
       <c r="AC44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -5825,8 +5849,11 @@
       <c r="AC45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5905,8 +5932,11 @@
       <c r="AC46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5988,8 +6018,11 @@
       <c r="AC47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6068,8 +6101,11 @@
       <c r="AC48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6148,8 +6184,11 @@
       <c r="AC49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6228,8 +6267,11 @@
       <c r="AC50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6308,8 +6350,11 @@
       <c r="AC51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6388,8 +6433,11 @@
       <c r="AC52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6468,8 +6516,11 @@
       <c r="AC53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6548,8 +6599,11 @@
       <c r="AC54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6628,8 +6682,11 @@
       <c r="AC55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6708,8 +6765,11 @@
       <c r="AC56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6791,8 +6851,11 @@
       <c r="AC57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6871,8 +6934,11 @@
       <c r="AC58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6951,8 +7017,11 @@
       <c r="AC59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -7034,8 +7103,11 @@
       <c r="AC60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7117,8 +7189,11 @@
       <c r="AC61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7200,8 +7275,11 @@
       <c r="AC62" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7280,8 +7358,11 @@
       <c r="AC63" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7360,8 +7441,11 @@
       <c r="AC64" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7440,8 +7524,11 @@
       <c r="AC65" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7523,8 +7610,11 @@
       <c r="AC66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7603,8 +7693,11 @@
       <c r="AC67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7686,8 +7779,11 @@
       <c r="AC68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7769,8 +7865,11 @@
       <c r="AC69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7849,8 +7948,11 @@
       <c r="AC70" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7932,8 +8034,11 @@
       <c r="AC71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -8012,8 +8117,11 @@
       <c r="AC72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -8095,8 +8203,11 @@
       <c r="AC73" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -8178,8 +8289,11 @@
       <c r="AC74" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8261,8 +8375,11 @@
       <c r="AC75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8341,8 +8458,11 @@
       <c r="AC76" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8422,6 +8542,9 @@
         <v>1</v>
       </c>
       <c r="AC77" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD77">
         <v>0</v>
       </c>
     </row>
@@ -8547,7 +8670,7 @@
       <c r="AF1" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="5" t="s">
         <v>471</v>
       </c>
     </row>
@@ -8642,7 +8765,7 @@
       <c r="AF2">
         <v>0</v>
       </c>
-      <c r="AG2" s="5">
+      <c r="AG2" s="4">
         <v>0</v>
       </c>
     </row>
@@ -8734,7 +8857,7 @@
       <c r="AF3">
         <v>1</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AG3" s="4">
         <v>1</v>
       </c>
     </row>
@@ -8826,7 +8949,7 @@
       <c r="AF4">
         <v>1</v>
       </c>
-      <c r="AG4" s="5">
+      <c r="AG4" s="4">
         <v>0</v>
       </c>
     </row>
@@ -8918,7 +9041,7 @@
       <c r="AF5">
         <v>1</v>
       </c>
-      <c r="AG5" s="5">
+      <c r="AG5" s="4">
         <v>1</v>
       </c>
     </row>
@@ -9010,7 +9133,7 @@
       <c r="AF6">
         <v>0</v>
       </c>
-      <c r="AG6" s="5">
+      <c r="AG6" s="4">
         <v>1</v>
       </c>
     </row>
@@ -9102,7 +9225,7 @@
       <c r="AF7">
         <v>0</v>
       </c>
-      <c r="AG7" s="5">
+      <c r="AG7" s="4">
         <v>1</v>
       </c>
     </row>
@@ -9197,7 +9320,7 @@
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8" s="5">
+      <c r="AG8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9292,7 +9415,7 @@
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9" s="5">
+      <c r="AG9" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9384,7 +9507,7 @@
       <c r="AF10">
         <v>1</v>
       </c>
-      <c r="AG10" s="5">
+      <c r="AG10" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9476,7 +9599,7 @@
       <c r="AF11">
         <v>0</v>
       </c>
-      <c r="AG11" s="5">
+      <c r="AG11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9568,7 +9691,7 @@
       <c r="AF12">
         <v>1</v>
       </c>
-      <c r="AG12" s="5">
+      <c r="AG12" s="4">
         <v>1</v>
       </c>
     </row>
@@ -9660,7 +9783,7 @@
       <c r="AF13">
         <v>0</v>
       </c>
-      <c r="AG13" s="5">
+      <c r="AG13" s="4">
         <v>1</v>
       </c>
     </row>
@@ -9752,7 +9875,7 @@
       <c r="AF14">
         <v>0</v>
       </c>
-      <c r="AG14" s="5">
+      <c r="AG14" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9844,7 +9967,7 @@
       <c r="AF15">
         <v>0</v>
       </c>
-      <c r="AG15" s="5">
+      <c r="AG15" s="4">
         <v>1</v>
       </c>
     </row>
@@ -9936,7 +10059,7 @@
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16" s="5">
+      <c r="AG16" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9953,7 +10076,7 @@
         <f>SUM(AF2:AF16)</f>
         <v>6</v>
       </c>
-      <c r="AG17" s="5">
+      <c r="AG17" s="4">
         <f>SUM(AG2:AG16)</f>
         <v>7</v>
       </c>
@@ -9968,794 +10091,812 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93534103-3A08-4765-923A-CC35D144117E}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="27" t="s">
         <v>472</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="27" t="s">
         <v>473</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27" t="s">
         <v>474</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="27" t="s">
         <v>475</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>15</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="16">
         <f>(L5+M6)/$B$3</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="18" t="s">
         <v>481</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="8" t="s">
+      <c r="M3" s="19"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="16">
         <f>(Q5+R6)/$B$3</f>
         <v>0.4</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="18" t="s">
         <v>477</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>1/(B3)^2*((B5*B6)+(C5*C6))</f>
         <v>0.50666666666666671</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f>1/(B3)^2*((B5*B7)+(C5*C7))</f>
         <v>0.52</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <f>1/(B3)^2*((B5*B8)+(C5*C8))</f>
         <v>0.50666666666666671</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="5" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="5" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>9</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
         <f>1/(B3)^2*((B6*B7)+(C6*C7))</f>
         <v>0.50666666666666671</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <f>1/(B3)^2*((B6*B8)+(C6*C8))</f>
         <v>0.50222222222222224</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="15" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>3</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="7">
         <v>4</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="15" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="4">
         <v>2</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="7">
         <v>4</v>
       </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>8</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <f>1/(B3)^2*((B7*B8)+(C7*C8))</f>
         <v>0.50666666666666671</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17" t="s">
+      <c r="I6" s="4"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="8">
         <v>3</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="9">
         <v>5</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="8">
         <v>5</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="9">
         <v>4</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>9</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>8</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="8" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="16">
         <f>(L10+M11)/$B$3</f>
         <v>0.6</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="18" t="s">
         <v>481</v>
       </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="8" t="s">
+      <c r="M8" s="19"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="16">
         <f>(Q10+R11)/$B$3</f>
         <v>0.93333333333333335</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="18" t="s">
         <v>479</v>
       </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="5" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="5" t="s">
+      <c r="N9" s="4"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R9" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="19" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="22" t="s">
         <v>489</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="15" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <v>3</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="7">
         <v>3</v>
       </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="15" t="s">
+      <c r="N10" s="4"/>
+      <c r="O10" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="4">
         <v>6</v>
       </c>
-      <c r="R10" s="14">
-        <v>1</v>
-      </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="R10" s="7">
+        <v>1</v>
+      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="12" t="s">
         <v>485</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17" t="s">
+      <c r="I11" s="4"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="8">
         <v>3</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="9">
         <v>6</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="17" t="s">
+      <c r="N11" s="4"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="Q11" s="17">
-        <v>1</v>
-      </c>
-      <c r="R11" s="18">
+      <c r="Q11" s="8">
+        <v>1</v>
+      </c>
+      <c r="R11" s="9">
         <v>8</v>
       </c>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="22" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="11">
         <f>(K3-F4)/(1-F4)</f>
         <v>5.405405405405396E-2</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="11">
         <f>(P8-H5)/(1-H5)</f>
         <v>0.8660714285714286</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="12">
         <f>(P3-G5)/(1-G5)</f>
         <v>-0.21621621621621628</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="22" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="11">
         <f>(K8-G4)/(1-G4)</f>
         <v>0.1666666666666666</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="11">
         <f>(P13-H5)/(1-H5)</f>
         <v>6.2499999999999958E-2</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="8" t="s">
+      <c r="H13" s="12"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="16">
         <f>(L15+M16)/$B$3</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="18" t="s">
         <v>481</v>
       </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="8" t="s">
+      <c r="M13" s="19"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="P13" s="9">
+      <c r="P13" s="16">
         <f>(Q15+R16)/$B$3</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="Q13" s="10" t="s">
+      <c r="Q13" s="18" t="s">
         <v>479</v>
       </c>
-      <c r="R13" s="11"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="22" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="11">
         <f>(K13-H4)/(1-H4)</f>
         <v>5.405405405405396E-2</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="5" t="s">
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="5" t="s">
+      <c r="N14" s="4"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="R14" s="14" t="s">
+      <c r="R14" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="15" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="4">
         <v>3</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="7">
         <v>4</v>
       </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="15" t="s">
+      <c r="N15" s="4"/>
+      <c r="O15" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="P15" s="5" t="s">
+      <c r="P15" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="Q15" s="5">
+      <c r="Q15" s="4">
         <v>3</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15" s="7">
         <v>3</v>
       </c>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="17" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="8">
         <v>3</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="9">
         <v>5</v>
       </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="17" t="s">
+      <c r="N16" s="4"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="8">
         <v>4</v>
       </c>
-      <c r="R16" s="18">
+      <c r="R16" s="9">
         <v>5</v>
       </c>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:R8"/>
     <mergeCell ref="P13:P14"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="J15:J16"/>
@@ -10767,24 +10908,6 @@
     <mergeCell ref="K13:K14"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="O3:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>